<commit_message>
jn: diccionarios de las bases 1 3 17 18 realizados, queda pendiente cambio evento -> descripcion, reglas de calidad y relaciones
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/resumen_bdd_2025-03-25.xlsx
+++ b/04_Entregable 2/previo/resumen_bdd_2025-03-25.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -629,7 +629,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +693,7 @@
       <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -716,7 +716,7 @@
       <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -739,7 +739,7 @@
       <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -927,7 +927,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
@@ -953,7 +953,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>43</v>
       </c>
@@ -1002,8 +1002,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B16" t="s">
@@ -1067,7 +1067,7 @@
       <c r="F18" t="s">
         <v>54</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1090,12 +1090,12 @@
       <c r="F19" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B20" t="s">
@@ -1117,8 +1117,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B21" t="s">
@@ -1140,8 +1140,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B22" t="s">
@@ -1163,8 +1163,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B23" t="s">
@@ -1186,8 +1186,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B24" t="s">

</xml_diff>